<commit_message>
envio de mail con adjunto desde bd
</commit_message>
<xml_diff>
--- a/Enviar Mail/enviarmail/enviarmail/bin/Debug/Cotizaciones.xlsx
+++ b/Enviar Mail/enviarmail/enviarmail/bin/Debug/Cotizaciones.xlsx
@@ -174,26 +174,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -203,6 +185,24 @@
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -223,20 +223,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>695327</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>438150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>19957</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1652895</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>714375</xdr:rowOff>
+      <xdr:rowOff>618150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="3 Imagen"/>
+        <xdr:cNvPr id="5" name="4 Imagen" descr="Neovia_Ss_BZL_QP_RVB.PNG"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -249,8 +249,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="19050"/>
-          <a:ext cx="1258207" cy="695325"/>
+          <a:off x="9553577" y="438150"/>
+          <a:ext cx="957568" cy="180000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -261,20 +261,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>12</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>32386</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>677546</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>16616</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>15150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="6 Imagen"/>
+        <xdr:cNvPr id="6" name="5 Imagen" descr="mc.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -287,8 +287,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8258175" y="32386"/>
-          <a:ext cx="1209675" cy="645160"/>
+          <a:off x="12" y="19050"/>
+          <a:ext cx="1254854" cy="720000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -607,76 +607,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="57" customHeight="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="29.25" customHeight="1">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
     </row>
     <row r="3" spans="1:8" ht="18.75">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="12" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="7">
         <f>SUM(F5:F10000)</f>
         <v>1740</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="5">
         <f>SUM(H5:H10000)</f>
         <v>870000</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="4" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>